<commit_message>
Quad bus part update
</commit_message>
<xml_diff>
--- a/uncertainty/Uncertainty_BOM.xlsx
+++ b/uncertainty/Uncertainty_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kateartz/Desktop/Uncertainty_updated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kateartz/Desktop/OAM/Uncertainty_updated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E37FF45-4960-6C4A-A1DA-FCD9AE8CD30E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93B12D5-1E9B-3B47-AAA5-AF54A1B28C26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{74E01C8B-A62F-6F41-B39E-1E078C6F872C}"/>
+    <workbookView xWindow="280" yWindow="1640" windowWidth="25600" windowHeight="15500" xr2:uid="{74E01C8B-A62F-6F41-B39E-1E078C6F872C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Designator</t>
   </si>
@@ -204,15 +204,6 @@
     <t>TO-252</t>
   </si>
   <si>
-    <t xml:space="preserve">Onsemi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC74ACT05DG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverters 5V CMOS Hex w/Open Drain </t>
-  </si>
-  <si>
     <t xml:space="preserve">SOIC-14 </t>
   </si>
   <si>
@@ -229,6 +220,12 @@
   </si>
   <si>
     <t>Mounting Hardware UNI BKT BRS N PL</t>
+  </si>
+  <si>
+    <t>SN74HCS125QBQARQ1</t>
+  </si>
+  <si>
+    <t>Automotive Schmitt-trigger inputs quadruple bus buffer gates with 3-state outputs 14-WQFN -40 to 125</t>
   </si>
 </sst>
 </file>
@@ -605,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EAC47E-2B08-7943-9E5D-6089BD3B5C2A}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +613,7 @@
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="81.5" customWidth="1"/>
+    <col min="6" max="6" width="87.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
@@ -772,13 +769,13 @@
         <v>633</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -934,10 +931,10 @@
         <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -977,16 +974,16 @@
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -1006,10 +1003,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
New LEDs and mounting hardware
</commit_message>
<xml_diff>
--- a/uncertainty/Uncertainty_BOM.xlsx
+++ b/uncertainty/Uncertainty_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kateartz/Desktop/OAM/Uncertainty_updated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kateartz/Desktop/OAM/Uncertainty-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93B12D5-1E9B-3B47-AAA5-AF54A1B28C26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B12977-5899-1C4B-8ACF-F54DC630683E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="1640" windowWidth="25600" windowHeight="15500" xr2:uid="{74E01C8B-A62F-6F41-B39E-1E078C6F872C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{74E01C8B-A62F-6F41-B39E-1E078C6F872C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Designator</t>
   </si>
@@ -150,24 +150,15 @@
     <t xml:space="preserve">SOD-123 </t>
   </si>
   <si>
-    <t xml:space="preserve">Keystone Electronics </t>
-  </si>
-  <si>
     <t>35RASMT2AHNTRX</t>
   </si>
   <si>
     <t xml:space="preserve">Phone Connectors 3.5mm SMT MONO T/R 3A CLOSED </t>
   </si>
   <si>
-    <t>APGA1602SEC-E-KA</t>
-  </si>
-  <si>
     <t>Kingbright</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard LEDs - SMD 1.6X0.2MM RA 624nm RED SMD LED </t>
-  </si>
-  <si>
     <t>LM1117IMPX-3.3_NOPB</t>
   </si>
   <si>
@@ -219,13 +210,25 @@
     <t>Do not include this component in assembly</t>
   </si>
   <si>
-    <t>Mounting Hardware UNI BKT BRS N PL</t>
-  </si>
-  <si>
-    <t>SN74HCS125QBQARQ1</t>
-  </si>
-  <si>
-    <t>Automotive Schmitt-trigger inputs quadruple bus buffer gates with 3-state outputs 14-WQFN -40 to 125</t>
+    <t>SN74HCS125QDRQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automotive Schmitt-trigger inputs quadruple bus buffer gates with 3-state outputs 14-SOIC -40 to 125 </t>
+  </si>
+  <si>
+    <t>APPA3010SURCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard LEDs - SMD 3x1mm SMD RA RED </t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>Terminals WP-SMRA SMD Block 7mm</t>
+  </si>
+  <si>
+    <t>Component should be mounted so screw hole faces left edge of board</t>
   </si>
 </sst>
 </file>
@@ -602,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EAC47E-2B08-7943-9E5D-6089BD3B5C2A}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +619,7 @@
     <col min="6" max="6" width="87.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="43" customWidth="1"/>
+    <col min="9" max="9" width="57.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -763,19 +766,22 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E6" s="4">
-        <v>633</v>
+        <v>7466303</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -792,10 +798,10 @@
         <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
         <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>29</v>
@@ -815,16 +821,16 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1608</v>
+        <v>64</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="H8" t="s">
         <v>29</v>
@@ -841,16 +847,16 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
         <v>29</v>
@@ -870,10 +876,10 @@
         <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="4">
         <v>1005</v>
@@ -925,16 +931,16 @@
         <v>102010428</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -948,16 +954,16 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
@@ -974,16 +980,16 @@
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -1003,10 +1009,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>29</v>

</xml_diff>